<commit_message>
Fix some error on material 13
</commit_message>
<xml_diff>
--- a/Excel动手实验室 - 材料/13 - 高级IF函数.xlsx
+++ b/Excel动手实验室 - 材料/13 - 高级IF函数.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\OfficeTraining\Excel动手实验室 - 材料\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18435" windowHeight="8100"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18434" windowHeight="8097"/>
   </bookViews>
   <sheets>
     <sheet name="IF函数" sheetId="1" r:id="rId1"/>
@@ -18,10 +13,10 @@
     <sheet name="嵌套IF 2" sheetId="4" r:id="rId4"/>
     <sheet name="带有AND或OR的IF" sheetId="5" r:id="rId5"/>
     <sheet name="COUNTIFS" sheetId="7" r:id="rId6"/>
-    <sheet name="SUMIFS2" sheetId="6" r:id="rId7"/>
+    <sheet name="SUMIFS" sheetId="6" r:id="rId7"/>
     <sheet name="AVERAGEIFS" sheetId="10" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="75">
   <si>
     <t>支出</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -65,10 +60,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>IF(C2&gt;B2, "超出预算", "未超出预算")</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>类别</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -121,14 +112,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>IF(B2="易碎", 750, 0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>IF(TRIM(B2)="易碎", 750, 0)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>学生</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -157,10 +140,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>IF(b2&gt;=90,"A",IF(B2&gt;=80,"b",IF(B2&gt;=70,"C",IF(B2&gt;=60,"D","E"))</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>销售额</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -339,6 +318,9 @@
   </si>
   <si>
     <t>IFERROR(AVERAGEIFS($D$2:$D$7,$B$2:$B$7,F5,$C$2:$C$7,G5),"不适用")</t>
+  </si>
+  <si>
+    <t>IF(B2&gt;=90,"A",IF(B2&gt;=80,"B",IF(B2&gt;=70,"C",IF(B2&gt;=60,"D","E"))</t>
   </si>
 </sst>
 </file>
@@ -346,14 +328,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ [$¥-804]* #,##0.00_ ;_ [$¥-804]* \-#,##0.00_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ [$¥-804]* #,##0_ ;_ [$¥-804]* \-#,##0_ ;_ [$¥-804]* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -361,7 +343,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -369,14 +351,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -385,14 +367,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -460,7 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1">
@@ -475,7 +457,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -486,9 +468,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Accent5" xfId="2" builtinId="45"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="强调文字颜色 5" xfId="2" builtinId="45"/>
+    <cellStyle name="百分比" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -758,7 +740,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -766,14 +748,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="2" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="2" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -837,11 +819,6 @@
         <v>1743.8</v>
       </c>
       <c r="D5" s="1"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -852,79 +829,67 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>10</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="C6" s="2"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -938,22 +903,22 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>73</v>
@@ -962,7 +927,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>89</v>
@@ -971,7 +936,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>92</v>
@@ -980,7 +945,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
         <v>87</v>
@@ -989,7 +954,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1004,44 +969,44 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.73046875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>33</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="2">
         <v>70000</v>
       </c>
       <c r="C2" s="2"/>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F2" s="2">
         <v>100000</v>
@@ -1052,14 +1017,14 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2">
         <v>125000</v>
       </c>
       <c r="C3" s="2"/>
       <c r="E3" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F3" s="2">
         <v>50000</v>
@@ -1070,14 +1035,14 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="2">
         <v>25000</v>
       </c>
       <c r="C4" s="2"/>
       <c r="E4" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="F4" s="2">
         <v>0</v>
@@ -1088,7 +1053,7 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="2">
         <v>80000</v>
@@ -1097,7 +1062,7 @@
     </row>
     <row r="7" spans="1:7">
       <c r="B7" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1112,33 +1077,33 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="6" max="6" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="I1">
         <v>90</v>
@@ -1146,7 +1111,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1">
         <v>83</v>
@@ -1162,7 +1127,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1">
         <v>69</v>
@@ -1178,7 +1143,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1">
         <v>83</v>
@@ -1194,7 +1159,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
         <v>92</v>
@@ -1210,18 +1175,18 @@
     </row>
     <row r="7" spans="1:9">
       <c r="B7" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="B9" s="5" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1236,41 +1201,41 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
-    <col min="4" max="4" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33.75" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1">
         <v>75</v>
@@ -1279,19 +1244,19 @@
         <v>490170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
         <v>24</v>
@@ -1300,19 +1265,19 @@
         <v>777380</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
         <v>97</v>
@@ -1321,19 +1286,19 @@
         <v>411070</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1">
         <v>63</v>
@@ -1342,19 +1307,19 @@
         <v>572430</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1">
         <v>88</v>
@@ -1365,10 +1330,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -1377,7 +1342,7 @@
         <v>727070</v>
       </c>
       <c r="F7" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1390,11 +1355,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
@@ -1402,33 +1365,33 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1">
         <v>75</v>
@@ -1437,19 +1400,19 @@
         <v>490170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
         <v>24</v>
@@ -1458,19 +1421,19 @@
         <v>777380</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
         <v>97</v>
@@ -1479,19 +1442,19 @@
         <v>411070</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1">
         <v>63</v>
@@ -1500,19 +1463,19 @@
         <v>572430</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1">
         <v>88</v>
@@ -1523,10 +1486,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -1535,7 +1498,7 @@
         <v>727070</v>
       </c>
       <c r="F7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1550,7 +1513,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="14.35"/>
   <cols>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
@@ -1558,33 +1521,33 @@
   <sheetData>
     <row r="1" spans="1:8" ht="32.25" customHeight="1">
       <c r="A1" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H1" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1">
         <v>75</v>
@@ -1593,19 +1556,19 @@
         <v>490170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H2" s="9"/>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" s="1">
         <v>24</v>
@@ -1614,19 +1577,19 @@
         <v>777380</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H3" s="9"/>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1">
         <v>97</v>
@@ -1635,19 +1598,19 @@
         <v>411070</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H4" s="9"/>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1">
         <v>63</v>
@@ -1656,19 +1619,19 @@
         <v>572430</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H5" s="9"/>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1">
         <v>88</v>
@@ -1679,10 +1642,10 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1">
         <v>25</v>
@@ -1693,12 +1656,12 @@
     </row>
     <row r="9" spans="1:8">
       <c r="D9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="D11" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>